<commit_message>
Add comprehensive hosting solutions and production-ready app versions - Add HOSTING_GUIDE.md with multiple hosting options (Local, Heroku, Railway, Docker, Cloud) - Add app_with_celery.py for Redis/Celery integration - Add app_with_redis_alt.py for Python threading alternative - Add host_local.py for production local hosting - Add deploy_heroku.py for Heroku deployment automation - Add database utilities (init_db.py, check_db.py) - Add test_app.py for simplified testing - Add start_full_app.bat for complete app startup - Update material.xlsx - Add test_screenshot.png from Selenium testing
</commit_message>
<xml_diff>
--- a/material.xlsx
+++ b/material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s50045833\Downloads\MOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA52F4A-14AB-42BC-89EA-7E36DEC54081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD70D98E-979D-4237-9822-95B0635C43CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,7 +793,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Clean up project: Remove unused and unnecessary files - Remove Python cache files (__pycache__) - Remove test files (test_screenshot.png, test_selenium.py, test_app.py) - Remove duplicate app files (app.py) - Remove unused utility files (check_db.py, init_db.py, migrations.py, monitoring.py) - Remove old deployment files (start_full_app.bat) - Remove obsolete script files (map_screenshot.py, map_screenshot_parallel.py, materials.py, backup.py, cleanup.py) - Remove Chrome profile directory - Keep only essential files for production deployment
</commit_message>
<xml_diff>
--- a/material.xlsx
+++ b/material.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s50045833\Downloads\MOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD70D98E-979D-4237-9822-95B0635C43CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AA4516-F2A0-439C-A4E2-78FFA106F3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9790" yWindow="-25710" windowWidth="38620" windowHeight="25100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="warehouse" sheetId="1" r:id="rId1"/>
-    <sheet name="region" sheetId="2" r:id="rId2"/>
-    <sheet name="transportation" sheetId="3" r:id="rId3"/>
+    <sheet name="Warehouse" sheetId="1" r:id="rId1"/>
+    <sheet name="Region" sheetId="2" r:id="rId2"/>
+    <sheet name="Transportation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,10 +839,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="6">
@@ -854,19 +854,19 @@
       <c r="E2" s="4">
         <v>-1.391329</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="6">
@@ -878,19 +878,19 @@
       <c r="E3" s="4">
         <v>-1.656155</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="6">
@@ -902,19 +902,19 @@
       <c r="E4" s="4">
         <v>-1.874296</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="6">
@@ -926,19 +926,19 @@
       <c r="E5" s="4">
         <v>-2.0495700000000001</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="6">
@@ -950,19 +950,19 @@
       <c r="E6" s="4">
         <v>-2.2396430000000001</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="6">
@@ -974,19 +974,19 @@
       <c r="E7" s="4">
         <v>-1.775577</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="6">
@@ -998,19 +998,19 @@
       <c r="E8" s="4">
         <v>-2.4751500000000002</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="6">
@@ -1022,19 +1022,19 @@
       <c r="E9" s="4">
         <v>-2.575189</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="6">
@@ -1046,19 +1046,19 @@
       <c r="E10" s="4">
         <v>-1.56809</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="6">
@@ -1070,19 +1070,19 @@
       <c r="E11" s="4">
         <v>-1.741368</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="6">
@@ -1094,19 +1094,19 @@
       <c r="E12" s="4">
         <v>-1.9018839999999999</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="6">
@@ -1118,19 +1118,19 @@
       <c r="E13" s="4">
         <v>-2.0256430000000001</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="6">
@@ -1142,19 +1142,19 @@
       <c r="E14" s="4">
         <v>-1.852174</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="6">
@@ -1166,19 +1166,19 @@
       <c r="E15" s="4">
         <v>-1.9602120000000001</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="6">
@@ -1190,19 +1190,19 @@
       <c r="E16" s="4">
         <v>-1.2060770000000001</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="6">
@@ -1214,19 +1214,19 @@
       <c r="E17" s="4">
         <v>-2.1004710000000002</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="6">
@@ -1238,19 +1238,19 @@
       <c r="E18" s="4">
         <v>-1.988685</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="F18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="6">
@@ -1262,19 +1262,19 @@
       <c r="E19" s="4">
         <v>-2.6301809999999999</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="6">
@@ -1286,19 +1286,19 @@
       <c r="E20" s="4">
         <v>-2.5597599999999998</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="6">
@@ -1310,19 +1310,19 @@
       <c r="E21" s="4">
         <v>-2.7924039999999999</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="F21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="6">
@@ -1334,19 +1334,19 @@
       <c r="E22" s="4">
         <v>-2.784478</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="2" t="s">
+      <c r="F22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="6">
@@ -1358,19 +1358,19 @@
       <c r="E23" s="4">
         <v>-2.728726</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="6">
@@ -1382,19 +1382,19 @@
       <c r="E24" s="4">
         <v>-2.6816070000000001</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="6">
@@ -1406,19 +1406,19 @@
       <c r="E25" s="4">
         <v>-2.570856</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="F25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="7">
@@ -1430,18 +1430,18 @@
       <c r="E26" s="5">
         <v>-2.2325699999999999</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="F26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="7">
@@ -1453,18 +1453,18 @@
       <c r="E27" s="5">
         <v>-2.9130790000000002</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="F27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="7">
@@ -1476,18 +1476,18 @@
       <c r="E28" s="5">
         <v>-2.1737199999999999</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="7">
@@ -1499,18 +1499,18 @@
       <c r="E29" s="5">
         <v>-2.9854530000000001</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="F29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="7">
@@ -1522,18 +1522,18 @@
       <c r="E30" s="5">
         <v>-3.0452710000000001</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="F30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="7">
@@ -1545,18 +1545,18 @@
       <c r="E31" s="5">
         <v>-2.3577780000000002</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="7">
@@ -1568,18 +1568,18 @@
       <c r="E32" s="5">
         <v>-2.277196</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="7">
@@ -1591,10 +1591,10 @@
       <c r="E33" s="5">
         <v>-2.10026</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix total routes display and job completion issues - Updated worker to properly set total_routes and complete jobs - Fixed database context issues in worker - Enhanced error handling and job retrieval - All completed jobs now show correct progress and download links
</commit_message>
<xml_diff>
--- a/material.xlsx
+++ b/material.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s50045833\Downloads\MOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AA4516-F2A0-439C-A4E2-78FFA106F3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5ED7DF-2D76-4F56-A33D-4B9E9EB95B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9790" yWindow="-25710" windowWidth="38620" windowHeight="25100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9790" yWindow="-25710" windowWidth="38620" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warehouse" sheetId="1" r:id="rId1"/>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,10 +578,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +793,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,10 +820,10 @@
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -1004,7 +1004,6 @@
       <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">

</xml_diff>